<commit_message>
documentación sprint 2 y 3
</commit_message>
<xml_diff>
--- a/Documentación/Sprints/AnalisisDiseño_Sprint2.xlsx
+++ b/Documentación/Sprints/AnalisisDiseño_Sprint2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Paula/ICI 2013/VIII Semestre/Taller Ing Software/RedDebate/Documentación/Sprints/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Paula/ICI 2013/VIII Semestre/Taller Ing Software/RedDebate/Documentación/Sprints/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="460" windowWidth="28500" windowHeight="16600" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1440" yWindow="460" windowWidth="25600" windowHeight="16700" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Análisis1 (2.1)" sheetId="4" r:id="rId1"/>
@@ -103,9 +103,6 @@
     <t>solicitud_cierre()</t>
   </si>
   <si>
-    <t>se solicitó el despliegue de menú con la información del usuario y el debate</t>
-  </si>
-  <si>
     <t>Solicitar el cierre del debate</t>
   </si>
   <si>
@@ -200,9 +197,6 @@
 el usuario es el creador del debate</t>
   </si>
   <si>
-    <t>se solicitó el despliegue del "pop up" de confirmación de cierre</t>
-  </si>
-  <si>
     <t>cerrar el debate, cambiando el estado de éste.</t>
   </si>
   <si>
@@ -220,9 +214,6 @@
 (2) se entegó la lista de los debates "cerrados"</t>
   </si>
   <si>
-    <t>Se cambió el estado del debate a "Cerrado"</t>
-  </si>
-  <si>
     <t>OBS: Se genera este caso de uso para avanzar en el caso de uso "definir postura"</t>
   </si>
   <si>
@@ -241,6 +232,15 @@
   </si>
   <si>
     <t>Diagrama de Colaboración</t>
+  </si>
+  <si>
+    <t>(1) Se cambió el estado del debate a "Cerrado"</t>
+  </si>
+  <si>
+    <t>(1) se solicitó el despliegue del "pop up" de confirmación de cierre</t>
+  </si>
+  <si>
+    <t>(1) se solicitó el despliegue de menú con la información del usuario y el debate</t>
   </si>
 </sst>
 </file>
@@ -485,86 +485,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -580,6 +523,63 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -793,6 +793,49 @@
         <a:xfrm>
           <a:off x="6672386" y="907307"/>
           <a:ext cx="4132384" cy="1909161"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="825500" y="1079500"/>
+          <a:ext cx="7962900" cy="1562100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1084,147 +1127,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" spans="2:6" ht="22" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="11"/>
-    </row>
-    <row r="2" spans="2:6" ht="22" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
+      <c r="F2" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="33"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="27"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16"/>
-      <c r="F2" s="42" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="19"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="22"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="21" t="s">
+      <c r="D5" s="27"/>
+    </row>
+    <row r="6" spans="2:6" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="22"/>
-    </row>
-    <row r="6" spans="2:6" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="21" t="s">
+      <c r="D6" s="27"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="27"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="22"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="22"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="22"/>
+      <c r="D8" s="27"/>
     </row>
     <row r="9" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="41"/>
     </row>
     <row r="10" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="2:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="31"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="43"/>
+      <c r="D12" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="28" t="s">
+    </row>
+    <row r="13" spans="2:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="B13" s="34" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="B13" s="29" t="s">
+      <c r="C13" s="35"/>
+      <c r="D13" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="8" t="s">
+    </row>
+    <row r="14" spans="2:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="B14" s="34" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="B14" s="29" t="s">
+      <c r="C14" s="35"/>
+      <c r="D14" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="8" t="s">
+    </row>
+    <row r="15" spans="2:6" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="36" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="31" t="s">
+      <c r="C15" s="37"/>
+      <c r="D15" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="33" t="s">
+    </row>
+    <row r="16" spans="2:6" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="19"/>
+    </row>
+    <row r="17" spans="2:4" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="31"/>
+    </row>
+    <row r="18" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="38" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="34"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="36"/>
-    </row>
-    <row r="17" spans="2:4" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16"/>
-    </row>
-    <row r="18" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="37" t="s">
+      <c r="C18" s="39"/>
+      <c r="D18" s="20" t="s">
         <v>47</v>
-      </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="39" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1239,12 +1282,12 @@
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1255,8 +1298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K45"/>
   <sheetViews>
-    <sheetView zoomScale="139" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="C14" zoomScale="139" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1270,11 +1313,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
@@ -1284,11 +1327,11 @@
       <c r="K1" s="11"/>
     </row>
     <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="E2" s="41" t="s">
+      <c r="C2" s="44"/>
+      <c r="E2" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1298,7 +1341,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="30" x14ac:dyDescent="0.2">
@@ -1306,7 +1349,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
@@ -1314,7 +1357,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
@@ -1346,7 +1389,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1354,12 +1397,12 @@
         <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
     </row>
     <row r="14" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:11" x14ac:dyDescent="0.2">
@@ -1375,7 +1418,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
@@ -1383,7 +1426,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
@@ -1415,7 +1458,7 @@
         <v>11</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1423,7 +1466,7 @@
         <v>10</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1434,8 +1477,8 @@
       <c r="C26" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="41" t="s">
-        <v>26</v>
+      <c r="E26" s="22" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
@@ -1443,7 +1486,7 @@
         <v>15</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
@@ -1451,7 +1494,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
@@ -1483,7 +1526,7 @@
         <v>11</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1491,7 +1534,7 @@
         <v>10</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1500,7 +1543,7 @@
         <v>16</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.2">
@@ -1508,7 +1551,7 @@
         <v>15</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.2">
@@ -1516,7 +1559,7 @@
         <v>3</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.2">
@@ -1554,7 +1597,7 @@
         <v>10</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1571,20 +1614,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="B1" s="43" t="s">
-        <v>49</v>
+      <c r="B1" s="24" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="2:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="B3" s="44" t="s">
-        <v>67</v>
+      <c r="B3" s="25" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1611,119 +1654,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="F1" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" ht="22" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
+      <c r="F2" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="33"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="27"/>
+    </row>
+    <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="27"/>
+    </row>
+    <row r="6" spans="2:6" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="27"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="F1" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="2:6" ht="22" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16"/>
-      <c r="F2" s="42" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="19"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="22"/>
-    </row>
-    <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="22"/>
-    </row>
-    <row r="6" spans="2:6" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="22"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="22"/>
+      <c r="D7" s="27"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="22"/>
+      <c r="C8" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="27"/>
     </row>
     <row r="9" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="41"/>
     </row>
     <row r="10" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="2:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="31"/>
     </row>
     <row r="12" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="43"/>
+      <c r="D12" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="28" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="13" spans="2:6" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="32"/>
+      <c r="B13" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="37"/>
       <c r="D13" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
@@ -1731,6 +1769,11 @@
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1742,7 +1785,7 @@
   <dimension ref="B1:K65"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1756,11 +1799,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
@@ -1770,11 +1813,11 @@
       <c r="K1" s="11"/>
     </row>
     <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="E2" s="41" t="s">
+      <c r="C2" s="44"/>
+      <c r="E2" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1784,7 +1827,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="30" x14ac:dyDescent="0.2">
@@ -1792,7 +1835,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
@@ -1800,7 +1843,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
@@ -1832,10 +1875,10 @@
         <v>11</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>10</v>
       </c>
@@ -2143,23 +2186,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B1:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="B1" s="43" t="s">
-        <v>27</v>
+      <c r="B1" s="24" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="2:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="B3" s="44" t="s">
-        <v>67</v>
+      <c r="B3" s="25" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>